<commit_message>
pom.xml is modified with selenium-server dependency
</commit_message>
<xml_diff>
--- a/src/test/java/XLFiles/Guru99BankTestData.xlsx
+++ b/src/test/java/XLFiles/Guru99BankTestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Customer Name</t>
   </si>
@@ -96,37 +96,16 @@
     <t>subhash.kiran@appistoki.com</t>
   </si>
   <si>
-    <t>23698</t>
-  </si>
-  <si>
-    <t>21063</t>
-  </si>
-  <si>
-    <t>77926</t>
-  </si>
-  <si>
-    <t>72182</t>
-  </si>
-  <si>
-    <t>34482</t>
-  </si>
-  <si>
-    <t>77294</t>
-  </si>
-  <si>
-    <t>51926</t>
-  </si>
-  <si>
-    <t>11049</t>
-  </si>
-  <si>
-    <t>69679</t>
-  </si>
-  <si>
-    <t>7998</t>
-  </si>
-  <si>
     <t>71920</t>
+  </si>
+  <si>
+    <t>subhash.kiran@gmail.com</t>
+  </si>
+  <si>
+    <t>8908</t>
+  </si>
+  <si>
+    <t>36475</t>
   </si>
 </sst>
 </file>
@@ -495,7 +474,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +547,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>14</v>
@@ -616,7 +595,7 @@
     <col min="7" max="7" bestFit="true" customWidth="true" width="9.87109375" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.6171875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="15.3671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.609375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -654,7 +633,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -679,7 +658,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>